<commit_message>
first succesfull tests w/ everythng(MILP,rnflw,GA)
</commit_message>
<xml_diff>
--- a/Tests/Test6/test_GA_DoD.xlsx
+++ b/Tests/Test6/test_GA_DoD.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abb-my.sharepoint.com/personal/pierfrancesco_losi_se_abb_com/Documents/Documents/Projects/Model/Tests/Test6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEPILOS\OneDrive - ABB\Documents\Projects\Model\Tests\Test6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_B6D468AD1B4E46D5DBBDD45A47543ABCBA225083" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD19FAC5-6B0A-4F07-9A57-56C112B6861C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306DE7C0-2002-49C2-8F9D-6F44E8E92FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Design Space" sheetId="2" r:id="rId2"/>
+    <sheet name="Design Space" sheetId="4" r:id="rId2"/>
     <sheet name="Objective Space" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -317,7 +317,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34C97622-2773-4D63-BDAE-512FF8928C1C}" type="CELLRANGE">
+                    <a:fld id="{DD55BF82-BC18-41F9-9696-5809B2FBA8F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -340,7 +340,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{00000000-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -351,7 +351,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{44C74388-019D-4D3D-AC7E-9BD2DD7E32BF}" type="CELLRANGE">
+                    <a:fld id="{A7445B6A-94EC-4FB1-A68C-72EF1133E9E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -374,7 +374,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{00000001-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -385,7 +385,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33CC018B-2AB0-4B1C-89DE-C396BEC55477}" type="CELLRANGE">
+                    <a:fld id="{902A0EC6-D182-48A1-AFFA-3422622B2D86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -408,7 +408,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{00000002-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -419,7 +419,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{237FCFCC-D0BB-46A2-99CD-29B2565DED2B}" type="CELLRANGE">
+                    <a:fld id="{A4ABEF28-E8DE-42ED-8912-2D1958856B8B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -442,7 +442,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{00000003-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -453,7 +453,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35AF19CC-B233-48F0-96E2-ED641CCACE81}" type="CELLRANGE">
+                    <a:fld id="{6CDDA441-3CAA-4307-B395-4D30D32F1255}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -476,7 +476,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{00000004-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -487,7 +487,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C493C666-6CC9-48F9-82AA-2B9D1BB66150}" type="CELLRANGE">
+                    <a:fld id="{1E9716A3-1451-474A-9F5A-E87737D98796}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -510,7 +510,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{00000005-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -521,7 +521,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{44668605-E51C-4FC4-85AB-1ECE63A8B936}" type="CELLRANGE">
+                    <a:fld id="{A13A35A8-26F1-4AD6-AFED-642774E2BA6F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -544,7 +544,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{00000006-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -555,7 +555,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C86B00C5-72C2-4F38-87D8-F67DA9833693}" type="CELLRANGE">
+                    <a:fld id="{E6D14A5B-462F-440D-B60E-35FF79877D3C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -578,7 +578,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{00000007-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -589,7 +589,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7FC0DAB7-79E1-425F-92D7-41F01E59D742}" type="CELLRANGE">
+                    <a:fld id="{CD1DB844-774D-4DFB-A19A-EE6538B34258}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -612,7 +612,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{00000008-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -623,7 +623,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E28F5E14-45CB-4E7F-B3AB-936A2E500A96}" type="CELLRANGE">
+                    <a:fld id="{112E5B9A-3AA5-47D8-A64C-A57FD1217F2C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -646,7 +646,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{00000009-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -657,7 +657,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FBFAC31D-F2FE-4EE3-B6E3-A57C4103BD26}" type="CELLRANGE">
+                    <a:fld id="{9F7F4C21-1539-4AEA-99BC-4413BEE831B9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -680,7 +680,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{0000000A-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -691,7 +691,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{43396839-65C6-4BFE-90F1-3A2B3BDAFE0F}" type="CELLRANGE">
+                    <a:fld id="{190F3CE3-5D21-4042-8AFF-9CB121632D5C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -714,7 +714,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000B-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{0000000B-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -725,7 +725,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6F74D40D-C21B-43C0-A371-1151CDFD1218}" type="CELLRANGE">
+                    <a:fld id="{8203EBE5-CA70-414F-8566-79536576DD83}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -748,7 +748,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000C-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{0000000C-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -759,7 +759,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63BE7988-6F46-413C-A73D-21808D8A6F94}" type="CELLRANGE">
+                    <a:fld id="{E9B3132F-0474-46A1-BE49-7707A5CCD32E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -782,7 +782,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000D-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{0000000D-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -793,7 +793,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F7392BC5-D282-4132-B4B6-7E5A12A09C28}" type="CELLRANGE">
+                    <a:fld id="{967B8338-C7ED-4C23-8C54-D857E1010A27}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -816,7 +816,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000E-8F11-43B2-A4E6-624EEB829D8F}"/>
+                  <c16:uniqueId val="{0000000E-B754-4EDA-B25A-A9FCBB1740D4}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1040,7 +1040,7 @@
               </c15:datalabelsRange>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-8F11-43B2-A4E6-624EEB829D8F}"/>
+              <c16:uniqueId val="{0000000F-B754-4EDA-B25A-A9FCBB1740D4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1482,7 +1482,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1BABD276-A064-4F86-B9DA-BDA7376428F1}" type="CELLRANGE">
+                    <a:fld id="{89B6F96E-95B5-4ECD-A9AA-19BAB97924EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1516,7 +1516,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F623CFB-243F-430C-8397-6324D2430B69}" type="CELLRANGE">
+                    <a:fld id="{24C2C805-40FD-45F3-94BD-96684DF8BC7F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1550,7 +1550,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D9EC66E5-3F6B-4BA7-83F5-6AA8C40B7938}" type="CELLRANGE">
+                    <a:fld id="{D4EB6715-F80C-4521-A5FE-D14238D351AB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1584,7 +1584,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{118364FC-DE3C-44B2-B265-6F0D69F260AB}" type="CELLRANGE">
+                    <a:fld id="{B12D3784-36A5-4D91-8BBC-43850F7D792A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1618,7 +1618,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7DC7A6FA-385D-4533-8300-F0CA794F9769}" type="CELLRANGE">
+                    <a:fld id="{73C248A8-21EE-428F-9360-1AA4AD4C372C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1652,7 +1652,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{62011EE8-619A-40E6-AB09-120AF76E72AD}" type="CELLRANGE">
+                    <a:fld id="{7AEAC137-EE2E-4AC3-A8C3-5FEEDF8C170D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1686,7 +1686,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9FCD60F-8F27-4B62-AEE4-C2867C6E8EA3}" type="CELLRANGE">
+                    <a:fld id="{C3510B7A-6E8A-4878-9689-23ECA10CB9C9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1720,7 +1720,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F216981-BE5B-4FED-9B1B-AC47B97B38A9}" type="CELLRANGE">
+                    <a:fld id="{EA22B1CE-8451-4BCD-B068-100219FB852B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1754,7 +1754,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1F5D37A-8A53-4CE4-A7BC-33CB9A1F6A63}" type="CELLRANGE">
+                    <a:fld id="{A1CD6C17-32AB-4D3D-91A1-AF70196D14DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1788,7 +1788,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4949CA91-C95C-40E3-B894-7DD4AEC715E9}" type="CELLRANGE">
+                    <a:fld id="{C9545AA5-9296-4AED-A443-165B1DE01995}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1822,7 +1822,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5581695-DCDD-4690-B439-0DA4DE09F0FF}" type="CELLRANGE">
+                    <a:fld id="{83FBBD84-C027-469C-BC80-7A2A74D65896}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1856,7 +1856,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CACED55B-466A-4457-8757-2D1EA336CDE2}" type="CELLRANGE">
+                    <a:fld id="{F4E3451F-4EDD-4107-AD1E-9AA48DE4691D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1890,7 +1890,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10BA8605-DE0C-4081-A04E-F02033FEDB40}" type="CELLRANGE">
+                    <a:fld id="{5E759D30-2FE8-40BA-9BE0-FD23437C032B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1924,7 +1924,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{980ADCE1-440E-4926-890F-B38EA548A55E}" type="CELLRANGE">
+                    <a:fld id="{8F135301-FD2B-44BE-AD87-EC4F489F7579}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1958,7 +1958,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C97C1AAC-D0D6-4E9F-9D51-B390A70846DE}" type="CELLRANGE">
+                    <a:fld id="{372DF709-3D19-4137-BC29-8B69C4F2917F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3625,10 +3625,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{28BAFEFE-683F-49B5-801D-EB4196B57FF4}">
-  <sheetPr/>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{DA93487C-DA12-4EF4-8401-05EB57615B1E}">
+  <sheetPr codeName="Chart2"/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3637,7 +3637,7 @@
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0CA9F41C-8C62-45F9-9DF8-4E7B8689C849}">
-  <sheetPr/>
+  <sheetPr codeName="Chart3"/>
   <sheetViews>
     <sheetView zoomScale="55" workbookViewId="0"/>
   </sheetViews>
@@ -3650,13 +3650,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9281438" cy="6054247"/>
+    <xdr:ext cx="9281438" cy="6045548"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CB94CB2-BA5A-BF7A-759B-E61AED301EF9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{773D51DB-3886-6273-572B-73AF2B797107}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3683,7 +3683,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9278471" cy="6058647"/>
+    <xdr:ext cx="9294091" cy="6049818"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3997,12 +3997,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>